<commit_message>
Did the same for the soda eval bis
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_eval/meta_data.xlsx
+++ b/scripts/projects/soda_eval/meta_data.xlsx
@@ -309,9 +309,6 @@
     <t>zl24</t>
   </si>
   <si>
-    <t>v2.2.58</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -442,6 +439,9 @@
   </si>
   <si>
     <t>Preliminary soda lakes data for evaluation</t>
+  </si>
+  <si>
+    <t>v2.2.38</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1135,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1210,6 +1210,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1583,7 +1589,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1624,6 +1630,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
@@ -1638,6 +1645,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="1">
@@ -2053,7 +2061,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BA8" sqref="BA8"/>
+      <selection pane="bottomRight" activeCell="AY13" sqref="AY13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2099,10 +2107,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="57" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>100</v>
       </c>
       <c r="F1" s="75" t="s">
         <v>2</v>
@@ -2111,31 +2119,31 @@
         <v>1</v>
       </c>
       <c r="H1" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I1" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="L1" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="M1" s="69" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="N1" s="69" t="s">
         <v>106</v>
-      </c>
-      <c r="N1" s="69" t="s">
-        <v>107</v>
       </c>
       <c r="O1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S1" s="15" t="s">
         <v>9</v>
@@ -2153,10 +2161,10 @@
         <v>71</v>
       </c>
       <c r="X1" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Y1" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z1" s="19" t="s">
         <v>15</v>
@@ -2281,41 +2289,41 @@
       <c r="B2" s="7"/>
       <c r="C2" s="8"/>
       <c r="D2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="76" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="58"/>
       <c r="H2" s="58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K2" s="62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L2" s="60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S2" s="16" t="s">
         <v>74</v>
@@ -2352,7 +2360,7 @@
       <c r="N3" s="80"/>
       <c r="O3" s="81"/>
       <c r="P3" s="81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R3" s="14" t="s">
         <v>8</v>
@@ -2364,22 +2372,22 @@
         <v>13</v>
       </c>
       <c r="U3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V3" t="s">
         <v>82</v>
       </c>
       <c r="W3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z3" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA3" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="AA3" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="AB3" s="25"/>
       <c r="AC3" s="25"/>
@@ -2404,10 +2412,10 @@
         <v>36</v>
       </c>
       <c r="AL3" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM3" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM3" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN3" s="21">
         <v>4</v>
@@ -2440,7 +2448,7 @@
         <v>51</v>
       </c>
       <c r="AX3" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY3" s="23">
         <v>100</v>
@@ -2470,10 +2478,10 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI3" t="s">
         <v>97</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>98</v>
       </c>
       <c r="BK3" s="23" t="s">
         <v>61</v>
@@ -2509,34 +2517,34 @@
       <c r="N4" s="85"/>
       <c r="O4" s="86"/>
       <c r="P4" s="86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="S4" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T4" s="22" t="s">
         <v>13</v>
       </c>
       <c r="U4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="W4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z4" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA4" s="25" t="s">
         <v>125</v>
-      </c>
-      <c r="AA4" s="25" t="s">
-        <v>126</v>
       </c>
       <c r="AB4" s="25"/>
       <c r="AC4" s="25"/>
@@ -2561,19 +2569,19 @@
         <v>36</v>
       </c>
       <c r="AL4" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM4" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM4" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN4" s="21">
         <v>4</v>
       </c>
       <c r="AO4" s="24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AP4" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AQ4" s="24">
         <v>2</v>
@@ -2597,7 +2605,7 @@
         <v>51</v>
       </c>
       <c r="AX4" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY4" s="23">
         <v>100</v>
@@ -2627,10 +2635,10 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI4" t="s">
         <v>97</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>98</v>
       </c>
       <c r="BK4" s="23" t="s">
         <v>61</v>
@@ -2666,7 +2674,7 @@
       <c r="N5" s="85"/>
       <c r="O5" s="86"/>
       <c r="P5" s="86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R5" s="14" t="s">
         <v>8</v>
@@ -2678,22 +2686,22 @@
         <v>13</v>
       </c>
       <c r="U5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V5" t="s">
         <v>83</v>
       </c>
       <c r="W5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z5" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA5" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="AA5" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="AB5" s="25"/>
       <c r="AC5" s="25"/>
@@ -2718,10 +2726,10 @@
         <v>36</v>
       </c>
       <c r="AL5" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM5" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM5" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN5" s="21">
         <v>4</v>
@@ -2754,7 +2762,7 @@
         <v>51</v>
       </c>
       <c r="AX5" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY5" s="23">
         <v>100</v>
@@ -2784,10 +2792,10 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH5" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI5" t="s">
         <v>97</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>98</v>
       </c>
       <c r="BK5" s="23" t="s">
         <v>61</v>
@@ -2835,7 +2843,7 @@
       </c>
       <c r="O6" s="86"/>
       <c r="P6" s="86" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R6" s="14" t="s">
         <v>8</v>
@@ -2847,22 +2855,22 @@
         <v>13</v>
       </c>
       <c r="U6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V6" t="s">
         <v>84</v>
       </c>
       <c r="W6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z6" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA6" s="25" t="s">
         <v>129</v>
-      </c>
-      <c r="AA6" s="25" t="s">
-        <v>130</v>
       </c>
       <c r="AB6" s="25"/>
       <c r="AC6" s="25"/>
@@ -2887,10 +2895,10 @@
         <v>36</v>
       </c>
       <c r="AL6" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM6" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM6" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN6" s="21">
         <v>4</v>
@@ -2923,7 +2931,7 @@
         <v>51</v>
       </c>
       <c r="AX6" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY6" s="23">
         <v>100</v>
@@ -2953,10 +2961,10 @@
         <v>16.780556000000001</v>
       </c>
       <c r="BH6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI6" t="s">
         <v>97</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>98</v>
       </c>
       <c r="BK6" s="23" t="s">
         <v>61</v>
@@ -3012,7 +3020,7 @@
         <v>329062500</v>
       </c>
       <c r="P7" s="81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="34"/>
       <c r="R7" s="14" t="s">
@@ -3025,22 +3033,22 @@
         <v>13</v>
       </c>
       <c r="U7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V7" s="34" t="s">
         <v>85</v>
       </c>
       <c r="W7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z7" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA7" s="25" t="s">
         <v>131</v>
-      </c>
-      <c r="AA7" s="25" t="s">
-        <v>132</v>
       </c>
       <c r="AB7" s="36"/>
       <c r="AC7" s="36"/>
@@ -3065,10 +3073,10 @@
         <v>36</v>
       </c>
       <c r="AL7" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM7" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM7" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN7" s="21">
         <v>4</v>
@@ -3101,7 +3109,7 @@
         <v>51</v>
       </c>
       <c r="AX7" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY7" s="23">
         <v>100</v>
@@ -3131,10 +3139,10 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH7" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI7" t="s">
         <v>97</v>
-      </c>
-      <c r="BI7" t="s">
-        <v>98</v>
       </c>
       <c r="BJ7" s="34"/>
       <c r="BK7" s="42" t="s">
@@ -3189,7 +3197,7 @@
         <v>281812500</v>
       </c>
       <c r="P8" s="86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q8" s="34"/>
       <c r="R8" s="14" t="s">
@@ -3202,22 +3210,22 @@
         <v>13</v>
       </c>
       <c r="U8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V8" s="34" t="s">
         <v>86</v>
       </c>
       <c r="W8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z8" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA8" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="AA8" s="25" t="s">
-        <v>134</v>
       </c>
       <c r="AB8" s="36"/>
       <c r="AC8" s="36"/>
@@ -3242,10 +3250,10 @@
         <v>36</v>
       </c>
       <c r="AL8" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM8" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM8" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN8" s="21">
         <v>4</v>
@@ -3278,7 +3286,7 @@
         <v>51</v>
       </c>
       <c r="AX8" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY8" s="23">
         <v>100</v>
@@ -3308,10 +3316,10 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH8" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI8" t="s">
         <v>97</v>
-      </c>
-      <c r="BI8" t="s">
-        <v>98</v>
       </c>
       <c r="BJ8" s="34"/>
       <c r="BK8" s="42" t="s">
@@ -3366,7 +3374,7 @@
         <v>81000000</v>
       </c>
       <c r="P9" s="86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q9" s="34"/>
       <c r="R9" s="14" t="s">
@@ -3379,22 +3387,22 @@
         <v>13</v>
       </c>
       <c r="U9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V9" s="34" t="s">
         <v>87</v>
       </c>
       <c r="W9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Z9" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA9" s="25" t="s">
         <v>135</v>
-      </c>
-      <c r="AA9" s="25" t="s">
-        <v>136</v>
       </c>
       <c r="AB9" s="36"/>
       <c r="AC9" s="36"/>
@@ -3419,10 +3427,10 @@
         <v>36</v>
       </c>
       <c r="AL9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM9" s="21" t="s">
         <v>139</v>
-      </c>
-      <c r="AM9" s="21" t="s">
-        <v>140</v>
       </c>
       <c r="AN9" s="21">
         <v>4</v>
@@ -3455,7 +3463,7 @@
         <v>51</v>
       </c>
       <c r="AX9" s="23" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY9" s="23">
         <v>100</v>
@@ -3485,10 +3493,10 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH9" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI9" t="s">
         <v>97</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>98</v>
       </c>
       <c r="BJ9" s="34"/>
       <c r="BK9" s="42" t="s">
@@ -3533,7 +3541,7 @@
       </c>
       <c r="O10" s="95"/>
       <c r="P10" s="95" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q10" s="44"/>
       <c r="R10" s="45" t="s">
@@ -3546,25 +3554,25 @@
         <v>13</v>
       </c>
       <c r="U10" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V10" s="44" t="s">
         <v>88</v>
       </c>
       <c r="W10" s="44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="X10" s="44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y10" s="44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Z10" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA10" s="48" t="s">
         <v>137</v>
-      </c>
-      <c r="AA10" s="48" t="s">
-        <v>138</v>
       </c>
       <c r="AB10" s="48"/>
       <c r="AC10" s="48"/>
@@ -3589,10 +3597,10 @@
         <v>36</v>
       </c>
       <c r="AL10" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="AM10" s="44" t="s">
         <v>139</v>
-      </c>
-      <c r="AM10" s="44" t="s">
-        <v>140</v>
       </c>
       <c r="AN10" s="54">
         <v>4</v>
@@ -3625,7 +3633,7 @@
         <v>51</v>
       </c>
       <c r="AX10" s="56" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="AY10" s="56">
         <v>100</v>
@@ -3655,10 +3663,10 @@
         <v>16.780833000000001</v>
       </c>
       <c r="BH10" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI10" s="44" t="s">
         <v>97</v>
-      </c>
-      <c r="BI10" s="44" t="s">
-        <v>98</v>
       </c>
       <c r="BJ10" s="44"/>
       <c r="BK10" s="56" t="s">
@@ -3681,6 +3689,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Update metadata integers for read counts
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_eval/meta_data.xlsx
+++ b/scripts/projects/soda_eval/meta_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="157">
   <si>
     <t>Sample</t>
   </si>
@@ -442,6 +442,54 @@
   </si>
   <si>
     <t>v2.2.38</t>
+  </si>
+  <si>
+    <t>359a090d1afe061bfc01b50dfa6e858b</t>
+  </si>
+  <si>
+    <t>44e8e605b9d4a42a118a24441f87364a</t>
+  </si>
+  <si>
+    <t>d851d8dbfe370ac068659fddb9c21812</t>
+  </si>
+  <si>
+    <t>445760d27be328717da2515d23875f4b</t>
+  </si>
+  <si>
+    <t>84382fb760336ac7d6315fbbf32b8c6f</t>
+  </si>
+  <si>
+    <t>2ee2460a6af40b41640b4f74d68a8268</t>
+  </si>
+  <si>
+    <t>f8fb2f8f18445b0fe7ebe1561e4795b1</t>
+  </si>
+  <si>
+    <t>834536a232530dcdcc29372d376deea9</t>
+  </si>
+  <si>
+    <t>51ab0592e54e719c7331a46ab335399b</t>
+  </si>
+  <si>
+    <t>644415116fbd7953acbd098482fde289</t>
+  </si>
+  <si>
+    <t>d803a56b1766fa875dd037b760e8cad0</t>
+  </si>
+  <si>
+    <t>27689afea850d7376c89b82f90dac833</t>
+  </si>
+  <si>
+    <t>c757a8a59bc9cf04c51f0ab69118cbc7</t>
+  </si>
+  <si>
+    <t>b6bb3c7cb72fa0bd52c20f1a99bd2976</t>
+  </si>
+  <si>
+    <t>d5465756ea2aaf19339dad3b6b1f015a</t>
+  </si>
+  <si>
+    <t>d60b7e31515bc7d8f54532c957a5497e</t>
   </si>
 </sst>
 </file>
@@ -2058,10 +2106,10 @@
   <dimension ref="A1:BL11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AY13" sqref="AY13"/>
+      <selection pane="bottomRight" activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2389,10 +2437,18 @@
       <c r="AA3" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
+      <c r="AB3" s="25">
+        <v>22022227</v>
+      </c>
+      <c r="AC3" s="25">
+        <v>22022227</v>
+      </c>
+      <c r="AD3" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE3" s="25" t="s">
+        <v>149</v>
+      </c>
       <c r="AF3" s="26" t="s">
         <v>33</v>
       </c>
@@ -2546,10 +2602,18 @@
       <c r="AA4" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
+      <c r="AB4" s="25">
+        <v>12526102</v>
+      </c>
+      <c r="AC4" s="25">
+        <v>12526102</v>
+      </c>
+      <c r="AD4" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>150</v>
+      </c>
       <c r="AF4" s="26" t="s">
         <v>33</v>
       </c>
@@ -2703,10 +2767,18 @@
       <c r="AA5" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
+      <c r="AB5" s="25">
+        <v>25312891</v>
+      </c>
+      <c r="AC5" s="25">
+        <v>25312891</v>
+      </c>
+      <c r="AD5" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE5" s="25" t="s">
+        <v>151</v>
+      </c>
       <c r="AF5" s="26" t="s">
         <v>33</v>
       </c>
@@ -2872,10 +2944,18 @@
       <c r="AA6" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
+      <c r="AB6" s="25">
+        <v>15542524</v>
+      </c>
+      <c r="AC6" s="25">
+        <v>15542524</v>
+      </c>
+      <c r="AD6" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE6" s="25" t="s">
+        <v>152</v>
+      </c>
       <c r="AF6" s="26" t="s">
         <v>33</v>
       </c>
@@ -3050,10 +3130,18 @@
       <c r="AA7" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="AB7" s="36"/>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="36"/>
+      <c r="AB7" s="36">
+        <v>42326105</v>
+      </c>
+      <c r="AC7" s="36">
+        <v>42326105</v>
+      </c>
+      <c r="AD7" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE7" s="36" t="s">
+        <v>153</v>
+      </c>
       <c r="AF7" s="37" t="s">
         <v>33</v>
       </c>
@@ -3227,10 +3315,18 @@
       <c r="AA8" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="AB8" s="36"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
+      <c r="AB8" s="36">
+        <v>12722007</v>
+      </c>
+      <c r="AC8" s="36">
+        <v>12722007</v>
+      </c>
+      <c r="AD8" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE8" s="36" t="s">
+        <v>154</v>
+      </c>
       <c r="AF8" s="37" t="s">
         <v>33</v>
       </c>
@@ -3404,10 +3500,18 @@
       <c r="AA9" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="AB9" s="36"/>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
+      <c r="AB9" s="36">
+        <v>20061376</v>
+      </c>
+      <c r="AC9" s="36">
+        <v>20061376</v>
+      </c>
+      <c r="AD9" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AE9" s="36" t="s">
+        <v>155</v>
+      </c>
       <c r="AF9" s="37" t="s">
         <v>33</v>
       </c>
@@ -3574,10 +3678,18 @@
       <c r="AA10" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="AB10" s="48"/>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="48"/>
-      <c r="AE10" s="48"/>
+      <c r="AB10" s="48">
+        <v>17396379</v>
+      </c>
+      <c r="AC10" s="48">
+        <v>17396379</v>
+      </c>
+      <c r="AD10" s="48" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE10" s="48" t="s">
+        <v>156</v>
+      </c>
       <c r="AF10" s="49" t="s">
         <v>33</v>
       </c>
@@ -3689,7 +3801,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added under_ice_rerun json files
</commit_message>
<xml_diff>
--- a/scripts/projects/soda_eval/meta_data.xlsx
+++ b/scripts/projects/soda_eval/meta_data.xlsx
@@ -1354,7 +1354,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1635,6 +1635,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="57">
@@ -2106,10 +2115,10 @@
   <dimension ref="A1:BL11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC13" sqref="AC13"/>
+      <selection pane="bottomRight" activeCell="AB3" sqref="AB3:AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2120,6 +2129,7 @@
     <col min="16" max="16" width="15" customWidth="1"/>
     <col min="20" max="20" width="13.1640625" customWidth="1"/>
     <col min="22" max="25" width="17.5" customWidth="1"/>
+    <col min="28" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13.83203125" customWidth="1"/>
     <col min="31" max="31" width="14.83203125" customWidth="1"/>
     <col min="33" max="33" width="15.33203125" customWidth="1"/>
@@ -2437,10 +2447,10 @@
       <c r="AA3" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="AB3" s="25">
+      <c r="AB3" s="103">
         <v>22022227</v>
       </c>
-      <c r="AC3" s="25">
+      <c r="AC3" s="103">
         <v>22022227</v>
       </c>
       <c r="AD3" s="25" t="s">
@@ -2602,10 +2612,10 @@
       <c r="AA4" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="AB4" s="25">
+      <c r="AB4" s="103">
         <v>12526102</v>
       </c>
-      <c r="AC4" s="25">
+      <c r="AC4" s="103">
         <v>12526102</v>
       </c>
       <c r="AD4" s="25" t="s">
@@ -2767,10 +2777,10 @@
       <c r="AA5" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AB5" s="25">
+      <c r="AB5" s="103">
         <v>25312891</v>
       </c>
-      <c r="AC5" s="25">
+      <c r="AC5" s="103">
         <v>25312891</v>
       </c>
       <c r="AD5" s="25" t="s">
@@ -2944,10 +2954,10 @@
       <c r="AA6" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="AB6" s="25">
+      <c r="AB6" s="103">
         <v>15542524</v>
       </c>
-      <c r="AC6" s="25">
+      <c r="AC6" s="103">
         <v>15542524</v>
       </c>
       <c r="AD6" s="25" t="s">
@@ -3130,10 +3140,10 @@
       <c r="AA7" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="AB7" s="36">
+      <c r="AB7" s="104">
         <v>42326105</v>
       </c>
-      <c r="AC7" s="36">
+      <c r="AC7" s="104">
         <v>42326105</v>
       </c>
       <c r="AD7" s="36" t="s">
@@ -3315,10 +3325,10 @@
       <c r="AA8" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="AB8" s="36">
+      <c r="AB8" s="104">
         <v>12722007</v>
       </c>
-      <c r="AC8" s="36">
+      <c r="AC8" s="104">
         <v>12722007</v>
       </c>
       <c r="AD8" s="36" t="s">
@@ -3500,10 +3510,10 @@
       <c r="AA9" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="AB9" s="36">
+      <c r="AB9" s="104">
         <v>20061376</v>
       </c>
-      <c r="AC9" s="36">
+      <c r="AC9" s="104">
         <v>20061376</v>
       </c>
       <c r="AD9" s="36" t="s">
@@ -3678,10 +3688,10 @@
       <c r="AA10" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="AB10" s="48">
+      <c r="AB10" s="105">
         <v>17396379</v>
       </c>
-      <c r="AC10" s="48">
+      <c r="AC10" s="105">
         <v>17396379</v>
       </c>
       <c r="AD10" s="48" t="s">

</xml_diff>